<commit_message>
finance async load list
</commit_message>
<xml_diff>
--- a/admin/assets/file/export/transaction.xlsx
+++ b/admin/assets/file/export/transaction.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1532">
   <si>
     <t>Transaction Report</t>
   </si>
@@ -3843,160 +3843,406 @@
     <t>2018-01-17 18:09:57</t>
   </si>
   <si>
-    <t>$101.07</t>
-  </si>
-  <si>
-    <t>$104.07</t>
-  </si>
-  <si>
-    <t>label fee for order - ID: 925  store order ID: Amazon</t>
-  </si>
-  <si>
-    <t>2018-01-18 10:53:13</t>
-  </si>
-  <si>
-    <t>$10.08</t>
-  </si>
-  <si>
-    <t>$13.08</t>
-  </si>
-  <si>
-    <t>2018-01-18 11:49:38</t>
-  </si>
-  <si>
-    <t>2018-01-18 12:50:46</t>
-  </si>
-  <si>
-    <t>2018-01-18 12:53:57</t>
-  </si>
-  <si>
-    <t>$155.29</t>
-  </si>
-  <si>
-    <t>$158.29</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:00:13</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:03:59</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:04:25</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:05:15</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:15:50</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:20:49</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:34:52</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:38:50</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:41:40</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:48:36</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:49:57</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:56:44</t>
-  </si>
-  <si>
-    <t>2018-01-18 13:59:26</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:01:13</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:02:48</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:09:04</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:14:47</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:22:37</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:30:44</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:31:13</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:33:56</t>
-  </si>
-  <si>
-    <t>2018-01-18 14:40:54</t>
-  </si>
-  <si>
-    <t>2018-01-18 15:34:53</t>
-  </si>
-  <si>
-    <t>2018-01-21 12:11:02</t>
-  </si>
-  <si>
-    <t>2018-01-21 12:11:56</t>
-  </si>
-  <si>
-    <t>2018-01-21 12:12:17</t>
-  </si>
-  <si>
-    <t>2018-01-21 16:22:56</t>
-  </si>
-  <si>
-    <t>2018-01-21 16:27:04</t>
-  </si>
-  <si>
-    <t>$80.86</t>
-  </si>
-  <si>
-    <t>$83.86</t>
-  </si>
-  <si>
-    <t>2018-01-21 16:29:23</t>
-  </si>
-  <si>
-    <t>2018-01-21 16:43:39</t>
-  </si>
-  <si>
-    <t>$101.31</t>
-  </si>
-  <si>
-    <t>$104.31</t>
-  </si>
-  <si>
-    <t>2018-01-23 10:16:36</t>
-  </si>
-  <si>
-    <t>$104.17</t>
-  </si>
-  <si>
-    <t>$107.17</t>
-  </si>
-  <si>
-    <t>2018-01-23 17:57:46</t>
-  </si>
-  <si>
-    <t>2018-01-23 18:08:16</t>
-  </si>
-  <si>
-    <t>2018-01-23 18:11:03</t>
-  </si>
-  <si>
-    <t>2018-01-23 18:13:49</t>
+    <t>$16.98</t>
+  </si>
+  <si>
+    <t>Order ID #920, Kou Lee, Fedex Tracking Number: 425087016999</t>
+  </si>
+  <si>
+    <t>2018-01-18 22:50:04</t>
+  </si>
+  <si>
+    <t>$18.86</t>
+  </si>
+  <si>
+    <t>$21.86</t>
+  </si>
+  <si>
+    <t>Order ID #921, Dario Linares, Fedex Tracking Number: 425087017002</t>
+  </si>
+  <si>
+    <t>2018-01-18 22:54:21</t>
+  </si>
+  <si>
+    <t>Order ID #922, Amina Perry, Fedex Tracking Number: 425087017013</t>
+  </si>
+  <si>
+    <t>2018-01-18 23:00:20</t>
+  </si>
+  <si>
+    <t>Order ID #923, Dale Campbell, Fedex Tracking Number: 425087017024</t>
+  </si>
+  <si>
+    <t>2018-01-18 23:05:04</t>
+  </si>
+  <si>
+    <t>$12.83</t>
+  </si>
+  <si>
+    <t>$15.83</t>
+  </si>
+  <si>
+    <t>Order ID #924, Art Brochet, Fedex Tracking Number: 425087017035</t>
+  </si>
+  <si>
+    <t>2018-01-18 23:08:08</t>
+  </si>
+  <si>
+    <t>$103.92</t>
+  </si>
+  <si>
+    <t>$106.92</t>
+  </si>
+  <si>
+    <t>Order ID #925, Lisa Kemp, Fedex Tracking Number: 425087017046</t>
+  </si>
+  <si>
+    <t>2018-01-18 23:21:09</t>
+  </si>
+  <si>
+    <t>Order ID #928, Irek Mirgaleev, Fedex Tracking Number: 425087017160</t>
+  </si>
+  <si>
+    <t>2018-01-19 22:10:52</t>
+  </si>
+  <si>
+    <t>$19.71</t>
+  </si>
+  <si>
+    <t>$21.71</t>
+  </si>
+  <si>
+    <t>Order ID #929, Brady Rodriguez, Fedex Tracking Number: 425087017219</t>
+  </si>
+  <si>
+    <t>2018-01-19 22:46:48</t>
+  </si>
+  <si>
+    <t>XINYI NINGBO</t>
+  </si>
+  <si>
+    <t>$68.83</t>
+  </si>
+  <si>
+    <t>$71.83</t>
+  </si>
+  <si>
+    <t>Order ID #927, Sung Kyung Kim, Fedex Tracking Number: 425087017127</t>
+  </si>
+  <si>
+    <t>2018-01-19 22:52:34</t>
+  </si>
+  <si>
+    <t>$23.71</t>
+  </si>
+  <si>
+    <t>$26.71</t>
+  </si>
+  <si>
+    <t>Order ID #930, Bryce E Hauch, Fedex Tracking Number: 425087017138</t>
+  </si>
+  <si>
+    <t>2018-01-19 22:54:55</t>
+  </si>
+  <si>
+    <t>$35.18</t>
+  </si>
+  <si>
+    <t>$38.18</t>
+  </si>
+  <si>
+    <t>Order ID #931, Peter F Ulrich, Fedex Tracking Number: 425087017220</t>
+  </si>
+  <si>
+    <t>2018-01-19 22:58:49</t>
+  </si>
+  <si>
+    <t>Order ID #932, Marello Harris, Fedex Tracking Number: 425087017230</t>
+  </si>
+  <si>
+    <t>2018-01-19 23:05:25</t>
+  </si>
+  <si>
+    <t>$32.45</t>
+  </si>
+  <si>
+    <t>$35.45</t>
+  </si>
+  <si>
+    <t>Order ID #933, Bryan Beard, Fedex Tracking Number: 425087017241</t>
+  </si>
+  <si>
+    <t>2018-01-19 23:08:07</t>
+  </si>
+  <si>
+    <t>Order ID #934, Rodnia Pacheo/Karina Mantilla, Fedex Tracking Number: 425087017252</t>
+  </si>
+  <si>
+    <t>2018-01-19 23:11:33</t>
+  </si>
+  <si>
+    <t>$14.88</t>
+  </si>
+  <si>
+    <t>$17.88</t>
+  </si>
+  <si>
+    <t>Order ID #935, Sandra Reynolds, Fedex Tracking Number: 425087017263</t>
+  </si>
+  <si>
+    <t>2018-01-19 23:14:23</t>
+  </si>
+  <si>
+    <t>$20.23</t>
+  </si>
+  <si>
+    <t>$23.23</t>
+  </si>
+  <si>
+    <t>Order ID #936, Dexter Briceno, Fedex Tracking Number: 425087017285</t>
+  </si>
+  <si>
+    <t>2018-01-20 00:34:56</t>
+  </si>
+  <si>
+    <t>$28.97</t>
+  </si>
+  <si>
+    <t>$31.97</t>
+  </si>
+  <si>
+    <t>Order ID #937, Louis B. Katzerman, Fedex Tracking Number: 425087017296</t>
+  </si>
+  <si>
+    <t>2018-01-20 00:37:28</t>
+  </si>
+  <si>
+    <t>$17.02</t>
+  </si>
+  <si>
+    <t>$21.02</t>
+  </si>
+  <si>
+    <t>Order ID #926, Denne Adams, Fedex Tracking Number: 425087017344</t>
+  </si>
+  <si>
+    <t>2018-01-22 18:21:42</t>
+  </si>
+  <si>
+    <t>$20.28</t>
+  </si>
+  <si>
+    <t>$23.28</t>
+  </si>
+  <si>
+    <t>Order ID #939, Yuxuan Wei, Fedex Tracking Number: 425087017366</t>
+  </si>
+  <si>
+    <t>2018-01-23 17:55:04</t>
+  </si>
+  <si>
+    <t>$32.53</t>
+  </si>
+  <si>
+    <t>$35.53</t>
+  </si>
+  <si>
+    <t>Order ID #941, Jan Doran, Fedex Tracking Number: 425087017377</t>
+  </si>
+  <si>
+    <t>2018-01-23 17:56:18</t>
+  </si>
+  <si>
+    <t>$29.04</t>
+  </si>
+  <si>
+    <t>$32.04</t>
+  </si>
+  <si>
+    <t>Order ID #942, Johnny Ramos, Fedex Tracking Number: 425087017388</t>
+  </si>
+  <si>
+    <t>2018-01-23 17:57:57</t>
+  </si>
+  <si>
+    <t>$14.92</t>
+  </si>
+  <si>
+    <t>$17.92</t>
+  </si>
+  <si>
+    <t>Order ID #943, Jordan Lorenzo, Fedex Tracking Number: 425087017399</t>
+  </si>
+  <si>
+    <t>2018-01-23 17:59:39</t>
+  </si>
+  <si>
+    <t>$36.02</t>
+  </si>
+  <si>
+    <t>$39.02</t>
+  </si>
+  <si>
+    <t>Order ID #945, Brian K Cook, Fedex Tracking Number: 425087017403</t>
+  </si>
+  <si>
+    <t>2018-01-23 18:01:42</t>
+  </si>
+  <si>
+    <t>Order ID #946, Jonathan Daws, Fedex Tracking Number: 425087017414</t>
+  </si>
+  <si>
+    <t>2018-01-23 18:03:51</t>
+  </si>
+  <si>
+    <t>$17.15</t>
+  </si>
+  <si>
+    <t>$21.15</t>
+  </si>
+  <si>
+    <t>Order ID #947, Senad B. Kasumovic, Fedex Tracking Number: 425087017436</t>
+  </si>
+  <si>
+    <t>2018-01-23 18:06:50</t>
+  </si>
+  <si>
+    <t>Order ID #948, Kaleb T Anderson, Fedex Tracking Number: 425087017447</t>
+  </si>
+  <si>
+    <t>2018-01-23 18:50:59</t>
+  </si>
+  <si>
+    <t>Order ID #949, Gerald Siebe, Fedex Tracking Number: 425087017458</t>
+  </si>
+  <si>
+    <t>2018-01-23 18:53:02</t>
+  </si>
+  <si>
+    <t>$12.49</t>
+  </si>
+  <si>
+    <t>$15.49</t>
+  </si>
+  <si>
+    <t>Order ID #950, Josefina Ulloa, Fedex Tracking Number: 425087017540</t>
+  </si>
+  <si>
+    <t>2018-01-23 18:57:58</t>
+  </si>
+  <si>
+    <t>$27.50</t>
+  </si>
+  <si>
+    <t>$30.50</t>
+  </si>
+  <si>
+    <t>Order ID #951, Jennifer Stroud, Fedex Tracking Number: 425087017550</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:11:01</t>
+  </si>
+  <si>
+    <t>Order ID #952, Martha Acuna, Fedex Tracking Number: 425087017561</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:13:46</t>
+  </si>
+  <si>
+    <t>Order ID #953, Courtney Newell, Fedex Tracking Number: 425087017572</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:15:56</t>
+  </si>
+  <si>
+    <t>Order ID #954, Nadege Andre, Fedex Tracking Number: 425087017583</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:18:40</t>
+  </si>
+  <si>
+    <t>Order ID #955, Daniel F Mullen III, Fedex Tracking Number: 425087017609</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:20:55</t>
+  </si>
+  <si>
+    <t>Order ID #956, Zhu Xiao Tong, Fedex Tracking Number: 425087017610</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:22:23</t>
+  </si>
+  <si>
+    <t>$24.76</t>
+  </si>
+  <si>
+    <t>$27.76</t>
+  </si>
+  <si>
+    <t>Order ID #957, Abdullah Alotaibi, Fedex Tracking Number: 425087017642</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:23:46</t>
+  </si>
+  <si>
+    <t>Order ID #958, Toni Cummaro, Fedex Tracking Number: 425087017778</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:43:12</t>
+  </si>
+  <si>
+    <t>$11.74</t>
+  </si>
+  <si>
+    <t>$14.74</t>
+  </si>
+  <si>
+    <t>Order ID #959, Zach Westall, Fedex Tracking Number: 425087017789</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:46:20</t>
+  </si>
+  <si>
+    <t>$13.62</t>
+  </si>
+  <si>
+    <t>$16.62</t>
+  </si>
+  <si>
+    <t>Order ID #962, Tana Flowers, Fedex Tracking Number: 425087017815</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:54:12</t>
+  </si>
+  <si>
+    <t>Order ID #960, Glenn Stuart Rockowitz, Fedex Tracking Number: 425087017790</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:55:42</t>
+  </si>
+  <si>
+    <t>$15.90</t>
+  </si>
+  <si>
+    <t>$18.90</t>
+  </si>
+  <si>
+    <t>Order ID #961, Charle A Grant, Fedex Tracking Number: 425087017804</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:56:21</t>
+  </si>
+  <si>
+    <t>$16.90</t>
+  </si>
+  <si>
+    <t>$19.90</t>
+  </si>
+  <si>
+    <t>Order ID #963, Gary Marcus, Fedex Tracking Number: 425087017826</t>
+  </si>
+  <si>
+    <t>2018-01-23 19:59:37</t>
   </si>
   <si>
     <t>$35.27</t>
@@ -4005,34 +4251,367 @@
     <t>$38.27</t>
   </si>
   <si>
-    <t>label fee for order - ID: 930  store order ID: 113-8101758-4483454</t>
-  </si>
-  <si>
-    <t>2018-01-25 10:41:49</t>
-  </si>
-  <si>
-    <t>$24.76</t>
-  </si>
-  <si>
-    <t>$27.76</t>
-  </si>
-  <si>
-    <t>label fee for order - ID: 960  store order ID: 114-9638223-4108214</t>
-  </si>
-  <si>
-    <t>2018-01-25 10:47:31</t>
-  </si>
-  <si>
-    <t>2018-01-25 10:56:32</t>
-  </si>
-  <si>
-    <t>2018-01-25 10:57:31</t>
+    <t>Order ID #964, Aleshia A Weldon, Fedex Tracking Number: 425087017837</t>
+  </si>
+  <si>
+    <t>2018-01-23 20:01:57</t>
+  </si>
+  <si>
+    <t>Order ID #965, Craig Parnell, Fedex Tracking Number: 425087017848</t>
+  </si>
+  <si>
+    <t>2018-01-23 21:07:42</t>
+  </si>
+  <si>
+    <t>Order ID #966, Jason Washburn, Fedex Tracking Number: 425087017859</t>
+  </si>
+  <si>
+    <t>2018-01-23 21:09:59</t>
+  </si>
+  <si>
+    <t>$10.88</t>
+  </si>
+  <si>
+    <t>$13.88</t>
+  </si>
+  <si>
+    <t>Order ID #967, Gretchen Carvajal, RIVER ISLANDS, Fedex Tracking Number: 425087017860</t>
+  </si>
+  <si>
+    <t>2018-01-23 21:11:59</t>
+  </si>
+  <si>
+    <t>$19.64</t>
+  </si>
+  <si>
+    <t>$22.64</t>
+  </si>
+  <si>
+    <t>Order ID #973, Stephen Decker, Fedex Tracking Number: 425087017892</t>
+  </si>
+  <si>
+    <t>2018-01-24 17:41:39</t>
+  </si>
+  <si>
+    <t>Order ID #974, Ronald L Sjoblom, Fedex Tracking Number: 425087017907</t>
+  </si>
+  <si>
+    <t>2018-01-24 17:45:40</t>
+  </si>
+  <si>
+    <t>Order ID #975, Robert Gorlick, Fedex Tracking Number: 425087017918</t>
+  </si>
+  <si>
+    <t>2018-01-24 17:48:29</t>
+  </si>
+  <si>
+    <t>Order ID #976, Edda Navarro, Fedex Tracking Number: 425087017929</t>
+  </si>
+  <si>
+    <t>2018-01-24 17:50:45</t>
+  </si>
+  <si>
+    <t>Order ID #977, Anthony Castro, Fedex Tracking Number: 425087017930</t>
+  </si>
+  <si>
+    <t>2018-01-24 17:53:15</t>
+  </si>
+  <si>
+    <t>Order ID #978, Manuel Sanchez, Fedex Tracking Number: 425087017940</t>
+  </si>
+  <si>
+    <t>2018-01-24 17:55:19</t>
+  </si>
+  <si>
+    <t>$49.25</t>
+  </si>
+  <si>
+    <t>$52.25</t>
+  </si>
+  <si>
+    <t>Order ID #979, Antonio Smith, USPS Tracking Number: 	9405503699300174669576</t>
+  </si>
+  <si>
+    <t>2018-01-24 17:58:12</t>
+  </si>
+  <si>
+    <t>$13.39</t>
+  </si>
+  <si>
+    <t>$16.39</t>
+  </si>
+  <si>
+    <t>Order ID #980, Sue QuakenBush, Fedex Tracking Number: 425087017951</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:02:14</t>
+  </si>
+  <si>
+    <t>Order ID #981, Ben Rodden, Fedex Tracking Number: 425087017962</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:04:31</t>
+  </si>
+  <si>
+    <t>Order ID #984, Camilia Martin, Fedex Tracking Number: 425087017973</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:22:07</t>
+  </si>
+  <si>
+    <t>Order ID #985, Jennifer Bagley, Fedex Tracking Number: 425087017984</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:24:19</t>
+  </si>
+  <si>
+    <t>Order ID #986, Andrew Carbuto, Fedex Tracking Number: 425087017995</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:26:02</t>
+  </si>
+  <si>
+    <t>Order ID #987, James Kuo, Fedex Tracking Number: 425087018009</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:27:49</t>
+  </si>
+  <si>
+    <t>$18.64</t>
+  </si>
+  <si>
+    <t>$21.64</t>
+  </si>
+  <si>
+    <t>Order ID #988, Ron J Barlow, Fedex Tracking Number: 425087018010</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:29:48</t>
+  </si>
+  <si>
+    <t>Order ID #989, Joanne Schaeder, Fedex Tracking Number: 425087018020</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:31:47</t>
+  </si>
+  <si>
+    <t>Order ID #990, Catherine Rouiller, Fedex Tracking Number: 425087018031</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:52:34</t>
+  </si>
+  <si>
+    <t>Order ID #991, Fernando Lopez, Fedex Tracking Number: 425087018042</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:54:11</t>
+  </si>
+  <si>
+    <t>Order ID #992, Forres Best Hooser, Fedex Tracking Number: 425087018053</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:55:45</t>
+  </si>
+  <si>
+    <t>Order ID #993, Jon Wood, Fedex Tracking Number: 425087018064</t>
+  </si>
+  <si>
+    <t>2018-01-24 18:57:05</t>
+  </si>
+  <si>
+    <t>Order ID #968, Brian Shacklewood, Fedex Tracking Number: 425087018075</t>
+  </si>
+  <si>
+    <t>2018-01-24 19:09:30</t>
+  </si>
+  <si>
+    <t>Order ID #969, Susan Brown, Fedex Tracking Number: 425087018086</t>
+  </si>
+  <si>
+    <t>2018-01-24 19:15:31</t>
+  </si>
+  <si>
+    <t>Order ID #970, Scott Newlon, Fedex Tracking Number: 425087018097</t>
+  </si>
+  <si>
+    <t>2018-01-24 19:16:30</t>
+  </si>
+  <si>
+    <t>Order ID #971, Yongxian Chen, Fedex Tracking Number: 425087018101</t>
+  </si>
+  <si>
+    <t>2018-01-24 19:19:13</t>
+  </si>
+  <si>
+    <t>Order ID #972, Thienna Ho, Fedex Tracking Number: 425087018112</t>
+  </si>
+  <si>
+    <t>2018-01-24 19:21:56</t>
+  </si>
+  <si>
+    <t>Order ID #994, Shelby Lewis, Fedex Tracking Number: 425087018123</t>
+  </si>
+  <si>
+    <t>2018-01-24 19:24:36</t>
+  </si>
+  <si>
+    <t>Order ID #982, Debra Barber, Fedex Tracking Number: 425087018292</t>
+  </si>
+  <si>
+    <t>2018-01-24 21:21:59</t>
+  </si>
+  <si>
+    <t>Order ID #983, James Maertz, Fedex Tracking Number: 425087018318</t>
+  </si>
+  <si>
+    <t>2018-01-24 21:25:02</t>
+  </si>
+  <si>
+    <t>$39.60</t>
+  </si>
+  <si>
+    <t>$42.60</t>
+  </si>
+  <si>
+    <t>Order ID #995, Ana Romero, USPS Tracking Number: 9405503699300174953255</t>
+  </si>
+  <si>
+    <t>2018-01-24 21:38:31</t>
+  </si>
+  <si>
+    <t>$16.13</t>
+  </si>
+  <si>
+    <t>$19.13</t>
+  </si>
+  <si>
+    <t>Order ID #996, Jessica Green, Fedex Tracking Number: 425087018330</t>
+  </si>
+  <si>
+    <t>2018-01-24 21:42:04</t>
+  </si>
+  <si>
+    <t>Order ID #997, Jesse Armitage, Fedex Tracking Number: 425087018340</t>
+  </si>
+  <si>
+    <t>2018-01-24 21:44:03</t>
+  </si>
+  <si>
+    <t>Order ID #998, Paul Nelson, Fedex Tracking Number: 425087018351</t>
+  </si>
+  <si>
+    <t>2018-01-24 21:46:03</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 999  store order ID: 114-9638223-4108214</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:18:10</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1000  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:29:38</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1001  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:29:41</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1002  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:29:53</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1003  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:29:56</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1004  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:29:59</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1005  store order ID: Shopify</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:32:59</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1006  store order ID: Shopify</t>
+  </si>
+  <si>
+    <t>2018-01-25 11:33:02</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1007  store order ID: 114-5987646-0828213</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:36:11</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1008  store order ID: 114-0417088-4009829</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:37:08</t>
+  </si>
+  <si>
+    <t>$20.15</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1009  store order ID: 111-9339449-7779446</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:37:47</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1011  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:37:50</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1010  store order ID: Ebay</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:37:53</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1012  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:37:56</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1013  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:40:58</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1017  store order ID: 114-2028140-0506603</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:41:01</t>
+  </si>
+  <si>
+    <t>label fee for order - ID: 1015  store order ID: Amazon</t>
+  </si>
+  <si>
+    <t>2018-01-26 13:41:04</t>
   </si>
   <si>
     <t>Total Amount</t>
   </si>
   <si>
-    <t>$26,005.58</t>
+    <t>$23,379.99</t>
   </si>
 </sst>
 </file>
@@ -4386,10 +4965,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F603"/>
+  <dimension ref="A1:F653"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="F603" sqref="F603"/>
+      <selection activeCell="F653" sqref="F653"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4398,7 +4977,7 @@
     <col min="2" max="2" width="9.283447" bestFit="true" customWidth="true" style="0"/>
     <col min="3" max="3" width="8.140869" bestFit="true" customWidth="true" style="0"/>
     <col min="4" max="4" width="9.283447" bestFit="true" customWidth="true" style="0"/>
-    <col min="5" max="5" width="78.980713" bestFit="true" customWidth="true" style="0"/>
+    <col min="5" max="5" width="100.118408" bestFit="true" customWidth="true" style="0"/>
     <col min="6" max="6" width="23.422852" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -15545,13 +16124,13 @@
         <v>10</v>
       </c>
       <c r="D558" t="s">
+        <v>553</v>
+      </c>
+      <c r="E558" t="s">
         <v>1276</v>
       </c>
-      <c r="E558" t="s">
+      <c r="F558" t="s">
         <v>1277</v>
-      </c>
-      <c r="F558" t="s">
-        <v>1278</v>
       </c>
     </row>
     <row r="559" spans="1:6">
@@ -15559,16 +16138,16 @@
         <v>504</v>
       </c>
       <c r="B559" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C559" t="s">
+        <v>10</v>
+      </c>
+      <c r="D559" t="s">
         <v>1279</v>
       </c>
-      <c r="C559" t="s">
-        <v>10</v>
-      </c>
-      <c r="D559" t="s">
+      <c r="E559" t="s">
         <v>1280</v>
-      </c>
-      <c r="E559" t="s">
-        <v>1267</v>
       </c>
       <c r="F559" t="s">
         <v>1281</v>
@@ -15579,19 +16158,19 @@
         <v>504</v>
       </c>
       <c r="B560" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="C560" t="s">
         <v>10</v>
       </c>
       <c r="D560" t="s">
-        <v>1276</v>
+        <v>1279</v>
       </c>
       <c r="E560" t="s">
-        <v>1277</v>
+        <v>1282</v>
       </c>
       <c r="F560" t="s">
-        <v>1282</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="561" spans="1:6">
@@ -15599,19 +16178,19 @@
         <v>504</v>
       </c>
       <c r="B561" t="s">
-        <v>1275</v>
+        <v>1278</v>
       </c>
       <c r="C561" t="s">
         <v>10</v>
       </c>
       <c r="D561" t="s">
-        <v>1276</v>
+        <v>1279</v>
       </c>
       <c r="E561" t="s">
-        <v>1277</v>
+        <v>1284</v>
       </c>
       <c r="F561" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="562" spans="1:6">
@@ -15619,19 +16198,19 @@
         <v>504</v>
       </c>
       <c r="B562" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="C562" t="s">
         <v>10</v>
       </c>
       <c r="D562" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="E562" t="s">
-        <v>1277</v>
+        <v>1288</v>
       </c>
       <c r="F562" t="s">
-        <v>1286</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="563" spans="1:6">
@@ -15639,19 +16218,19 @@
         <v>504</v>
       </c>
       <c r="B563" t="s">
-        <v>1284</v>
+        <v>1290</v>
       </c>
       <c r="C563" t="s">
         <v>10</v>
       </c>
       <c r="D563" t="s">
-        <v>1285</v>
+        <v>1291</v>
       </c>
       <c r="E563" t="s">
-        <v>1277</v>
+        <v>1292</v>
       </c>
       <c r="F563" t="s">
-        <v>1287</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="564" spans="1:6">
@@ -15659,19 +16238,19 @@
         <v>504</v>
       </c>
       <c r="B564" t="s">
-        <v>1284</v>
+        <v>1278</v>
       </c>
       <c r="C564" t="s">
         <v>10</v>
       </c>
       <c r="D564" t="s">
-        <v>1285</v>
+        <v>1279</v>
       </c>
       <c r="E564" t="s">
-        <v>1277</v>
+        <v>1294</v>
       </c>
       <c r="F564" t="s">
-        <v>1288</v>
+        <v>1295</v>
       </c>
     </row>
     <row r="565" spans="1:6">
@@ -15679,199 +16258,199 @@
         <v>504</v>
       </c>
       <c r="B565" t="s">
-        <v>1284</v>
+        <v>1296</v>
       </c>
       <c r="C565" t="s">
         <v>10</v>
       </c>
       <c r="D565" t="s">
-        <v>1285</v>
+        <v>1297</v>
       </c>
       <c r="E565" t="s">
-        <v>1277</v>
+        <v>1298</v>
       </c>
       <c r="F565" t="s">
-        <v>1289</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="566" spans="1:6">
       <c r="A566" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B566" t="s">
-        <v>1284</v>
+        <v>1301</v>
       </c>
       <c r="C566" t="s">
         <v>10</v>
       </c>
       <c r="D566" t="s">
-        <v>1285</v>
+        <v>1302</v>
       </c>
       <c r="E566" t="s">
-        <v>1277</v>
+        <v>1303</v>
       </c>
       <c r="F566" t="s">
-        <v>1290</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="567" spans="1:6">
       <c r="A567" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B567" t="s">
-        <v>1284</v>
+        <v>1305</v>
       </c>
       <c r="C567" t="s">
         <v>10</v>
       </c>
       <c r="D567" t="s">
-        <v>1285</v>
+        <v>1306</v>
       </c>
       <c r="E567" t="s">
-        <v>1277</v>
+        <v>1307</v>
       </c>
       <c r="F567" t="s">
-        <v>1291</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="568" spans="1:6">
       <c r="A568" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B568" t="s">
-        <v>1284</v>
+        <v>1309</v>
       </c>
       <c r="C568" t="s">
         <v>10</v>
       </c>
       <c r="D568" t="s">
-        <v>1285</v>
+        <v>1310</v>
       </c>
       <c r="E568" t="s">
-        <v>1277</v>
+        <v>1311</v>
       </c>
       <c r="F568" t="s">
-        <v>1292</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="569" spans="1:6">
       <c r="A569" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B569" t="s">
-        <v>1284</v>
+        <v>1309</v>
       </c>
       <c r="C569" t="s">
         <v>10</v>
       </c>
       <c r="D569" t="s">
-        <v>1285</v>
+        <v>1310</v>
       </c>
       <c r="E569" t="s">
-        <v>1277</v>
+        <v>1313</v>
       </c>
       <c r="F569" t="s">
-        <v>1293</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="570" spans="1:6">
       <c r="A570" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B570" t="s">
-        <v>1284</v>
+        <v>1315</v>
       </c>
       <c r="C570" t="s">
         <v>10</v>
       </c>
       <c r="D570" t="s">
-        <v>1285</v>
+        <v>1316</v>
       </c>
       <c r="E570" t="s">
-        <v>1277</v>
+        <v>1317</v>
       </c>
       <c r="F570" t="s">
-        <v>1294</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="571" spans="1:6">
       <c r="A571" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B571" t="s">
-        <v>1284</v>
+        <v>1315</v>
       </c>
       <c r="C571" t="s">
         <v>10</v>
       </c>
       <c r="D571" t="s">
-        <v>1285</v>
+        <v>1316</v>
       </c>
       <c r="E571" t="s">
-        <v>1277</v>
+        <v>1319</v>
       </c>
       <c r="F571" t="s">
-        <v>1295</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="572" spans="1:6">
       <c r="A572" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B572" t="s">
-        <v>1284</v>
+        <v>1321</v>
       </c>
       <c r="C572" t="s">
         <v>10</v>
       </c>
       <c r="D572" t="s">
-        <v>1285</v>
+        <v>1322</v>
       </c>
       <c r="E572" t="s">
-        <v>1277</v>
+        <v>1323</v>
       </c>
       <c r="F572" t="s">
-        <v>1296</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="573" spans="1:6">
       <c r="A573" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B573" t="s">
-        <v>1284</v>
+        <v>1325</v>
       </c>
       <c r="C573" t="s">
         <v>10</v>
       </c>
       <c r="D573" t="s">
-        <v>1285</v>
+        <v>1326</v>
       </c>
       <c r="E573" t="s">
-        <v>1277</v>
+        <v>1327</v>
       </c>
       <c r="F573" t="s">
-        <v>1297</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="574" spans="1:6">
       <c r="A574" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B574" t="s">
-        <v>1284</v>
+        <v>1329</v>
       </c>
       <c r="C574" t="s">
         <v>10</v>
       </c>
       <c r="D574" t="s">
-        <v>1285</v>
+        <v>1330</v>
       </c>
       <c r="E574" t="s">
-        <v>1277</v>
+        <v>1331</v>
       </c>
       <c r="F574" t="s">
-        <v>1298</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="575" spans="1:6">
@@ -15879,379 +16458,379 @@
         <v>504</v>
       </c>
       <c r="B575" t="s">
-        <v>1284</v>
+        <v>1333</v>
       </c>
       <c r="C575" t="s">
         <v>10</v>
       </c>
       <c r="D575" t="s">
-        <v>1285</v>
+        <v>1334</v>
       </c>
       <c r="E575" t="s">
-        <v>1277</v>
+        <v>1335</v>
       </c>
       <c r="F575" t="s">
-        <v>1299</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="576" spans="1:6">
       <c r="A576" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B576" t="s">
-        <v>1275</v>
+        <v>1337</v>
       </c>
       <c r="C576" t="s">
         <v>10</v>
       </c>
       <c r="D576" t="s">
-        <v>1276</v>
+        <v>1338</v>
       </c>
       <c r="E576" t="s">
-        <v>1277</v>
+        <v>1339</v>
       </c>
       <c r="F576" t="s">
-        <v>1300</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="577" spans="1:6">
       <c r="A577" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B577" t="s">
-        <v>1275</v>
+        <v>1341</v>
       </c>
       <c r="C577" t="s">
         <v>10</v>
       </c>
       <c r="D577" t="s">
-        <v>1276</v>
+        <v>1342</v>
       </c>
       <c r="E577" t="s">
-        <v>1277</v>
+        <v>1343</v>
       </c>
       <c r="F577" t="s">
-        <v>1301</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="578" spans="1:6">
       <c r="A578" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B578" t="s">
-        <v>1275</v>
+        <v>1345</v>
       </c>
       <c r="C578" t="s">
         <v>10</v>
       </c>
       <c r="D578" t="s">
-        <v>1276</v>
+        <v>1346</v>
       </c>
       <c r="E578" t="s">
-        <v>1277</v>
+        <v>1347</v>
       </c>
       <c r="F578" t="s">
-        <v>1302</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="579" spans="1:6">
       <c r="A579" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B579" t="s">
-        <v>1275</v>
+        <v>1349</v>
       </c>
       <c r="C579" t="s">
         <v>10</v>
       </c>
       <c r="D579" t="s">
-        <v>1276</v>
+        <v>1350</v>
       </c>
       <c r="E579" t="s">
-        <v>1277</v>
+        <v>1351</v>
       </c>
       <c r="F579" t="s">
-        <v>1303</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="580" spans="1:6">
       <c r="A580" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B580" t="s">
-        <v>1275</v>
+        <v>1353</v>
       </c>
       <c r="C580" t="s">
         <v>10</v>
       </c>
       <c r="D580" t="s">
-        <v>1276</v>
+        <v>1354</v>
       </c>
       <c r="E580" t="s">
-        <v>1277</v>
+        <v>1355</v>
       </c>
       <c r="F580" t="s">
-        <v>1304</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="581" spans="1:6">
       <c r="A581" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B581" t="s">
-        <v>1275</v>
+        <v>1341</v>
       </c>
       <c r="C581" t="s">
         <v>10</v>
       </c>
       <c r="D581" t="s">
-        <v>1276</v>
+        <v>1342</v>
       </c>
       <c r="E581" t="s">
-        <v>1277</v>
+        <v>1357</v>
       </c>
       <c r="F581" t="s">
-        <v>1305</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="582" spans="1:6">
       <c r="A582" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B582" t="s">
-        <v>1275</v>
+        <v>1359</v>
       </c>
       <c r="C582" t="s">
         <v>10</v>
       </c>
       <c r="D582" t="s">
-        <v>1276</v>
+        <v>1360</v>
       </c>
       <c r="E582" t="s">
-        <v>1277</v>
+        <v>1361</v>
       </c>
       <c r="F582" t="s">
-        <v>1306</v>
+        <v>1362</v>
       </c>
     </row>
     <row r="583" spans="1:6">
       <c r="A583" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B583" t="s">
-        <v>1275</v>
+        <v>1353</v>
       </c>
       <c r="C583" t="s">
         <v>10</v>
       </c>
       <c r="D583" t="s">
-        <v>1276</v>
+        <v>1354</v>
       </c>
       <c r="E583" t="s">
-        <v>1277</v>
+        <v>1363</v>
       </c>
       <c r="F583" t="s">
-        <v>1307</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="584" spans="1:6">
       <c r="A584" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B584" t="s">
-        <v>1275</v>
+        <v>1341</v>
       </c>
       <c r="C584" t="s">
         <v>10</v>
       </c>
       <c r="D584" t="s">
-        <v>1276</v>
+        <v>1342</v>
       </c>
       <c r="E584" t="s">
-        <v>1277</v>
+        <v>1365</v>
       </c>
       <c r="F584" t="s">
-        <v>1308</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="585" spans="1:6">
       <c r="A585" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B585" t="s">
-        <v>1275</v>
+        <v>1367</v>
       </c>
       <c r="C585" t="s">
         <v>10</v>
       </c>
       <c r="D585" t="s">
-        <v>1276</v>
+        <v>1368</v>
       </c>
       <c r="E585" t="s">
-        <v>1277</v>
+        <v>1369</v>
       </c>
       <c r="F585" t="s">
-        <v>1309</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="586" spans="1:6">
       <c r="A586" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B586" t="s">
-        <v>1275</v>
+        <v>1371</v>
       </c>
       <c r="C586" t="s">
         <v>10</v>
       </c>
       <c r="D586" t="s">
-        <v>1276</v>
+        <v>1372</v>
       </c>
       <c r="E586" t="s">
-        <v>1277</v>
+        <v>1373</v>
       </c>
       <c r="F586" t="s">
-        <v>1310</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="587" spans="1:6">
       <c r="A587" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B587" t="s">
-        <v>1275</v>
+        <v>1341</v>
       </c>
       <c r="C587" t="s">
         <v>10</v>
       </c>
       <c r="D587" t="s">
-        <v>1276</v>
+        <v>1342</v>
       </c>
       <c r="E587" t="s">
-        <v>1277</v>
+        <v>1375</v>
       </c>
       <c r="F587" t="s">
-        <v>1311</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="588" spans="1:6">
       <c r="A588" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B588" t="s">
-        <v>1275</v>
+        <v>1345</v>
       </c>
       <c r="C588" t="s">
         <v>10</v>
       </c>
       <c r="D588" t="s">
-        <v>1276</v>
+        <v>1346</v>
       </c>
       <c r="E588" t="s">
-        <v>1277</v>
+        <v>1377</v>
       </c>
       <c r="F588" t="s">
-        <v>1312</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="589" spans="1:6">
       <c r="A589" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B589" t="s">
-        <v>1275</v>
+        <v>1341</v>
       </c>
       <c r="C589" t="s">
         <v>10</v>
       </c>
       <c r="D589" t="s">
-        <v>1276</v>
+        <v>1342</v>
       </c>
       <c r="E589" t="s">
-        <v>1277</v>
+        <v>1379</v>
       </c>
       <c r="F589" t="s">
-        <v>1313</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="590" spans="1:6">
       <c r="A590" t="s">
-        <v>8</v>
+        <v>1300</v>
       </c>
       <c r="B590" t="s">
-        <v>1314</v>
+        <v>1341</v>
       </c>
       <c r="C590" t="s">
         <v>10</v>
       </c>
       <c r="D590" t="s">
-        <v>1315</v>
+        <v>1342</v>
       </c>
       <c r="E590" t="s">
-        <v>1033</v>
+        <v>1381</v>
       </c>
       <c r="F590" t="s">
-        <v>1316</v>
+        <v>1382</v>
       </c>
     </row>
     <row r="591" spans="1:6">
       <c r="A591" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B591" t="s">
-        <v>1275</v>
+        <v>1341</v>
       </c>
       <c r="C591" t="s">
         <v>10</v>
       </c>
       <c r="D591" t="s">
-        <v>1276</v>
+        <v>1342</v>
       </c>
       <c r="E591" t="s">
-        <v>1277</v>
+        <v>1383</v>
       </c>
       <c r="F591" t="s">
-        <v>1317</v>
+        <v>1384</v>
       </c>
     </row>
     <row r="592" spans="1:6">
       <c r="A592" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B592" t="s">
-        <v>1318</v>
+        <v>1385</v>
       </c>
       <c r="C592" t="s">
         <v>10</v>
       </c>
       <c r="D592" t="s">
-        <v>1319</v>
+        <v>1386</v>
       </c>
       <c r="E592" t="s">
-        <v>1277</v>
+        <v>1387</v>
       </c>
       <c r="F592" t="s">
-        <v>1320</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="593" spans="1:6">
       <c r="A593" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B593" t="s">
-        <v>1321</v>
+        <v>1341</v>
       </c>
       <c r="C593" t="s">
         <v>10</v>
       </c>
       <c r="D593" t="s">
-        <v>1322</v>
+        <v>1342</v>
       </c>
       <c r="E593" t="s">
-        <v>1277</v>
+        <v>1389</v>
       </c>
       <c r="F593" t="s">
-        <v>1323</v>
+        <v>1390</v>
       </c>
     </row>
     <row r="594" spans="1:6">
@@ -16259,19 +16838,19 @@
         <v>504</v>
       </c>
       <c r="B594" t="s">
-        <v>1321</v>
+        <v>1391</v>
       </c>
       <c r="C594" t="s">
         <v>10</v>
       </c>
       <c r="D594" t="s">
-        <v>1322</v>
+        <v>1392</v>
       </c>
       <c r="E594" t="s">
-        <v>1277</v>
+        <v>1393</v>
       </c>
       <c r="F594" t="s">
-        <v>1324</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="595" spans="1:6">
@@ -16279,19 +16858,19 @@
         <v>504</v>
       </c>
       <c r="B595" t="s">
-        <v>1321</v>
+        <v>1395</v>
       </c>
       <c r="C595" t="s">
         <v>10</v>
       </c>
       <c r="D595" t="s">
-        <v>1322</v>
+        <v>1396</v>
       </c>
       <c r="E595" t="s">
-        <v>1277</v>
+        <v>1397</v>
       </c>
       <c r="F595" t="s">
-        <v>1325</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="596" spans="1:6">
@@ -16299,107 +16878,1107 @@
         <v>504</v>
       </c>
       <c r="B596" t="s">
-        <v>1321</v>
+        <v>1391</v>
       </c>
       <c r="C596" t="s">
         <v>10</v>
       </c>
       <c r="D596" t="s">
-        <v>1322</v>
+        <v>1392</v>
       </c>
       <c r="E596" t="s">
-        <v>1277</v>
+        <v>1399</v>
       </c>
       <c r="F596" t="s">
-        <v>1326</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="597" spans="1:6">
       <c r="A597" t="s">
-        <v>8</v>
+        <v>504</v>
       </c>
       <c r="B597" t="s">
-        <v>1327</v>
+        <v>1401</v>
       </c>
       <c r="C597" t="s">
         <v>10</v>
       </c>
       <c r="D597" t="s">
-        <v>1328</v>
+        <v>1402</v>
       </c>
       <c r="E597" t="s">
-        <v>1329</v>
+        <v>1403</v>
       </c>
       <c r="F597" t="s">
-        <v>1330</v>
+        <v>1404</v>
       </c>
     </row>
     <row r="598" spans="1:6">
       <c r="A598" t="s">
-        <v>8</v>
+        <v>504</v>
       </c>
       <c r="B598" t="s">
-        <v>1331</v>
+        <v>1405</v>
       </c>
       <c r="C598" t="s">
         <v>10</v>
       </c>
       <c r="D598" t="s">
-        <v>1332</v>
+        <v>1406</v>
       </c>
       <c r="E598" t="s">
-        <v>1333</v>
+        <v>1407</v>
       </c>
       <c r="F598" t="s">
-        <v>1334</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="599" spans="1:6">
       <c r="A599" t="s">
-        <v>8</v>
+        <v>1300</v>
       </c>
       <c r="B599" t="s">
-        <v>1331</v>
+        <v>1409</v>
       </c>
       <c r="C599" t="s">
         <v>10</v>
       </c>
       <c r="D599" t="s">
-        <v>1332</v>
+        <v>1410</v>
       </c>
       <c r="E599" t="s">
-        <v>1333</v>
+        <v>1411</v>
       </c>
       <c r="F599" t="s">
-        <v>1335</v>
+        <v>1412</v>
       </c>
     </row>
     <row r="600" spans="1:6">
       <c r="A600" t="s">
-        <v>504</v>
+        <v>1300</v>
       </c>
       <c r="B600" t="s">
-        <v>1321</v>
+        <v>1345</v>
       </c>
       <c r="C600" t="s">
         <v>10</v>
       </c>
       <c r="D600" t="s">
-        <v>1322</v>
+        <v>1346</v>
       </c>
       <c r="E600" t="s">
-        <v>1277</v>
+        <v>1413</v>
       </c>
       <c r="F600" t="s">
-        <v>1336</v>
+        <v>1414</v>
+      </c>
+    </row>
+    <row r="601" spans="1:6">
+      <c r="A601" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B601" t="s">
+        <v>1341</v>
+      </c>
+      <c r="C601" t="s">
+        <v>10</v>
+      </c>
+      <c r="D601" t="s">
+        <v>1342</v>
+      </c>
+      <c r="E601" t="s">
+        <v>1415</v>
+      </c>
+      <c r="F601" t="s">
+        <v>1416</v>
+      </c>
+    </row>
+    <row r="602" spans="1:6">
+      <c r="A602" t="s">
+        <v>504</v>
+      </c>
+      <c r="B602" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C602" t="s">
+        <v>10</v>
+      </c>
+      <c r="D602" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E602" t="s">
+        <v>1419</v>
+      </c>
+      <c r="F602" t="s">
+        <v>1420</v>
       </c>
     </row>
     <row r="603" spans="1:6">
-      <c r="E603" s="1" t="s">
-        <v>1337</v>
-      </c>
-      <c r="F603" s="1" t="s">
-        <v>1338</v>
+      <c r="A603" t="s">
+        <v>504</v>
+      </c>
+      <c r="B603" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C603" t="s">
+        <v>10</v>
+      </c>
+      <c r="D603" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E603" t="s">
+        <v>1423</v>
+      </c>
+      <c r="F603" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="604" spans="1:6">
+      <c r="A604" t="s">
+        <v>504</v>
+      </c>
+      <c r="B604" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C604" t="s">
+        <v>10</v>
+      </c>
+      <c r="D604" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E604" t="s">
+        <v>1425</v>
+      </c>
+      <c r="F604" t="s">
+        <v>1426</v>
+      </c>
+    </row>
+    <row r="605" spans="1:6">
+      <c r="A605" t="s">
+        <v>504</v>
+      </c>
+      <c r="B605" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C605" t="s">
+        <v>10</v>
+      </c>
+      <c r="D605" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E605" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F605" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="606" spans="1:6">
+      <c r="A606" t="s">
+        <v>504</v>
+      </c>
+      <c r="B606" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C606" t="s">
+        <v>10</v>
+      </c>
+      <c r="D606" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E606" t="s">
+        <v>1429</v>
+      </c>
+      <c r="F606" t="s">
+        <v>1430</v>
+      </c>
+    </row>
+    <row r="607" spans="1:6">
+      <c r="A607" t="s">
+        <v>504</v>
+      </c>
+      <c r="B607" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C607" t="s">
+        <v>10</v>
+      </c>
+      <c r="D607" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E607" t="s">
+        <v>1431</v>
+      </c>
+      <c r="F607" t="s">
+        <v>1432</v>
+      </c>
+    </row>
+    <row r="608" spans="1:6">
+      <c r="A608" t="s">
+        <v>504</v>
+      </c>
+      <c r="B608" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C608" t="s">
+        <v>10</v>
+      </c>
+      <c r="D608" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E608" t="s">
+        <v>1433</v>
+      </c>
+      <c r="F608" t="s">
+        <v>1434</v>
+      </c>
+    </row>
+    <row r="609" spans="1:6">
+      <c r="A609" t="s">
+        <v>504</v>
+      </c>
+      <c r="B609" t="s">
+        <v>1435</v>
+      </c>
+      <c r="C609" t="s">
+        <v>10</v>
+      </c>
+      <c r="D609" t="s">
+        <v>1436</v>
+      </c>
+      <c r="E609" t="s">
+        <v>1437</v>
+      </c>
+      <c r="F609" t="s">
+        <v>1438</v>
+      </c>
+    </row>
+    <row r="610" spans="1:6">
+      <c r="A610" t="s">
+        <v>504</v>
+      </c>
+      <c r="B610" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C610" t="s">
+        <v>10</v>
+      </c>
+      <c r="D610" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E610" t="s">
+        <v>1441</v>
+      </c>
+      <c r="F610" t="s">
+        <v>1442</v>
+      </c>
+    </row>
+    <row r="611" spans="1:6">
+      <c r="A611" t="s">
+        <v>504</v>
+      </c>
+      <c r="B611" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C611" t="s">
+        <v>10</v>
+      </c>
+      <c r="D611" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E611" t="s">
+        <v>1443</v>
+      </c>
+      <c r="F611" t="s">
+        <v>1444</v>
+      </c>
+    </row>
+    <row r="612" spans="1:6">
+      <c r="A612" t="s">
+        <v>504</v>
+      </c>
+      <c r="B612" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C612" t="s">
+        <v>10</v>
+      </c>
+      <c r="D612" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E612" t="s">
+        <v>1445</v>
+      </c>
+      <c r="F612" t="s">
+        <v>1446</v>
+      </c>
+    </row>
+    <row r="613" spans="1:6">
+      <c r="A613" t="s">
+        <v>504</v>
+      </c>
+      <c r="B613" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C613" t="s">
+        <v>10</v>
+      </c>
+      <c r="D613" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E613" t="s">
+        <v>1447</v>
+      </c>
+      <c r="F613" t="s">
+        <v>1448</v>
+      </c>
+    </row>
+    <row r="614" spans="1:6">
+      <c r="A614" t="s">
+        <v>504</v>
+      </c>
+      <c r="B614" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C614" t="s">
+        <v>10</v>
+      </c>
+      <c r="D614" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E614" t="s">
+        <v>1449</v>
+      </c>
+      <c r="F614" t="s">
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="615" spans="1:6">
+      <c r="A615" t="s">
+        <v>504</v>
+      </c>
+      <c r="B615" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C615" t="s">
+        <v>10</v>
+      </c>
+      <c r="D615" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E615" t="s">
+        <v>1451</v>
+      </c>
+      <c r="F615" t="s">
+        <v>1452</v>
+      </c>
+    </row>
+    <row r="616" spans="1:6">
+      <c r="A616" t="s">
+        <v>504</v>
+      </c>
+      <c r="B616" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C616" t="s">
+        <v>10</v>
+      </c>
+      <c r="D616" t="s">
+        <v>1454</v>
+      </c>
+      <c r="E616" t="s">
+        <v>1455</v>
+      </c>
+      <c r="F616" t="s">
+        <v>1456</v>
+      </c>
+    </row>
+    <row r="617" spans="1:6">
+      <c r="A617" t="s">
+        <v>504</v>
+      </c>
+      <c r="B617" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C617" t="s">
+        <v>10</v>
+      </c>
+      <c r="D617" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E617" t="s">
+        <v>1457</v>
+      </c>
+      <c r="F617" t="s">
+        <v>1458</v>
+      </c>
+    </row>
+    <row r="618" spans="1:6">
+      <c r="A618" t="s">
+        <v>504</v>
+      </c>
+      <c r="B618" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C618" t="s">
+        <v>10</v>
+      </c>
+      <c r="D618" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E618" t="s">
+        <v>1459</v>
+      </c>
+      <c r="F618" t="s">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="619" spans="1:6">
+      <c r="A619" t="s">
+        <v>504</v>
+      </c>
+      <c r="B619" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C619" t="s">
+        <v>10</v>
+      </c>
+      <c r="D619" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E619" t="s">
+        <v>1461</v>
+      </c>
+      <c r="F619" t="s">
+        <v>1462</v>
+      </c>
+    </row>
+    <row r="620" spans="1:6">
+      <c r="A620" t="s">
+        <v>504</v>
+      </c>
+      <c r="B620" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C620" t="s">
+        <v>10</v>
+      </c>
+      <c r="D620" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E620" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F620" t="s">
+        <v>1464</v>
+      </c>
+    </row>
+    <row r="621" spans="1:6">
+      <c r="A621" t="s">
+        <v>504</v>
+      </c>
+      <c r="B621" t="s">
+        <v>1401</v>
+      </c>
+      <c r="C621" t="s">
+        <v>10</v>
+      </c>
+      <c r="D621" t="s">
+        <v>1402</v>
+      </c>
+      <c r="E621" t="s">
+        <v>1465</v>
+      </c>
+      <c r="F621" t="s">
+        <v>1466</v>
+      </c>
+    </row>
+    <row r="622" spans="1:6">
+      <c r="A622" t="s">
+        <v>504</v>
+      </c>
+      <c r="B622" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C622" t="s">
+        <v>10</v>
+      </c>
+      <c r="D622" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E622" t="s">
+        <v>1467</v>
+      </c>
+      <c r="F622" t="s">
+        <v>1468</v>
+      </c>
+    </row>
+    <row r="623" spans="1:6">
+      <c r="A623" t="s">
+        <v>504</v>
+      </c>
+      <c r="B623" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C623" t="s">
+        <v>10</v>
+      </c>
+      <c r="D623" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E623" t="s">
+        <v>1469</v>
+      </c>
+      <c r="F623" t="s">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="624" spans="1:6">
+      <c r="A624" t="s">
+        <v>504</v>
+      </c>
+      <c r="B624" t="s">
+        <v>1453</v>
+      </c>
+      <c r="C624" t="s">
+        <v>10</v>
+      </c>
+      <c r="D624" t="s">
+        <v>1454</v>
+      </c>
+      <c r="E624" t="s">
+        <v>1471</v>
+      </c>
+      <c r="F624" t="s">
+        <v>1472</v>
+      </c>
+    </row>
+    <row r="625" spans="1:6">
+      <c r="A625" t="s">
+        <v>504</v>
+      </c>
+      <c r="B625" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C625" t="s">
+        <v>10</v>
+      </c>
+      <c r="D625" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E625" t="s">
+        <v>1473</v>
+      </c>
+      <c r="F625" t="s">
+        <v>1474</v>
+      </c>
+    </row>
+    <row r="626" spans="1:6">
+      <c r="A626" t="s">
+        <v>504</v>
+      </c>
+      <c r="B626" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C626" t="s">
+        <v>10</v>
+      </c>
+      <c r="D626" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E626" t="s">
+        <v>1475</v>
+      </c>
+      <c r="F626" t="s">
+        <v>1476</v>
+      </c>
+    </row>
+    <row r="627" spans="1:6">
+      <c r="A627" t="s">
+        <v>504</v>
+      </c>
+      <c r="B627" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C627" t="s">
+        <v>10</v>
+      </c>
+      <c r="D627" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E627" t="s">
+        <v>1477</v>
+      </c>
+      <c r="F627" t="s">
+        <v>1478</v>
+      </c>
+    </row>
+    <row r="628" spans="1:6">
+      <c r="A628" t="s">
+        <v>504</v>
+      </c>
+      <c r="B628" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C628" t="s">
+        <v>10</v>
+      </c>
+      <c r="D628" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E628" t="s">
+        <v>1479</v>
+      </c>
+      <c r="F628" t="s">
+        <v>1480</v>
+      </c>
+    </row>
+    <row r="629" spans="1:6">
+      <c r="A629" t="s">
+        <v>504</v>
+      </c>
+      <c r="B629" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C629" t="s">
+        <v>10</v>
+      </c>
+      <c r="D629" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E629" t="s">
+        <v>1481</v>
+      </c>
+      <c r="F629" t="s">
+        <v>1482</v>
+      </c>
+    </row>
+    <row r="630" spans="1:6">
+      <c r="A630" t="s">
+        <v>504</v>
+      </c>
+      <c r="B630" t="s">
+        <v>1483</v>
+      </c>
+      <c r="C630" t="s">
+        <v>10</v>
+      </c>
+      <c r="D630" t="s">
+        <v>1484</v>
+      </c>
+      <c r="E630" t="s">
+        <v>1485</v>
+      </c>
+      <c r="F630" t="s">
+        <v>1486</v>
+      </c>
+    </row>
+    <row r="631" spans="1:6">
+      <c r="A631" t="s">
+        <v>504</v>
+      </c>
+      <c r="B631" t="s">
+        <v>1487</v>
+      </c>
+      <c r="C631" t="s">
+        <v>10</v>
+      </c>
+      <c r="D631" t="s">
+        <v>1488</v>
+      </c>
+      <c r="E631" t="s">
+        <v>1489</v>
+      </c>
+      <c r="F631" t="s">
+        <v>1490</v>
+      </c>
+    </row>
+    <row r="632" spans="1:6">
+      <c r="A632" t="s">
+        <v>504</v>
+      </c>
+      <c r="B632" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C632" t="s">
+        <v>10</v>
+      </c>
+      <c r="D632" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E632" t="s">
+        <v>1491</v>
+      </c>
+      <c r="F632" t="s">
+        <v>1492</v>
+      </c>
+    </row>
+    <row r="633" spans="1:6">
+      <c r="A633" t="s">
+        <v>504</v>
+      </c>
+      <c r="B633" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C633" t="s">
+        <v>10</v>
+      </c>
+      <c r="D633" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E633" t="s">
+        <v>1493</v>
+      </c>
+      <c r="F633" t="s">
+        <v>1494</v>
+      </c>
+    </row>
+    <row r="634" spans="1:6">
+      <c r="A634" t="s">
+        <v>8</v>
+      </c>
+      <c r="B634" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C634" t="s">
+        <v>10</v>
+      </c>
+      <c r="D634" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E634" t="s">
+        <v>1495</v>
+      </c>
+      <c r="F634" t="s">
+        <v>1496</v>
+      </c>
+    </row>
+    <row r="635" spans="1:6">
+      <c r="A635" t="s">
+        <v>504</v>
+      </c>
+      <c r="B635" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C635" t="s">
+        <v>10</v>
+      </c>
+      <c r="D635" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E635" t="s">
+        <v>1497</v>
+      </c>
+      <c r="F635" t="s">
+        <v>1498</v>
+      </c>
+    </row>
+    <row r="636" spans="1:6">
+      <c r="A636" t="s">
+        <v>504</v>
+      </c>
+      <c r="B636" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C636" t="s">
+        <v>10</v>
+      </c>
+      <c r="D636" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E636" t="s">
+        <v>1499</v>
+      </c>
+      <c r="F636" t="s">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="637" spans="1:6">
+      <c r="A637" t="s">
+        <v>504</v>
+      </c>
+      <c r="B637" t="s">
+        <v>1391</v>
+      </c>
+      <c r="C637" t="s">
+        <v>10</v>
+      </c>
+      <c r="D637" t="s">
+        <v>1392</v>
+      </c>
+      <c r="E637" t="s">
+        <v>1501</v>
+      </c>
+      <c r="F637" t="s">
+        <v>1502</v>
+      </c>
+    </row>
+    <row r="638" spans="1:6">
+      <c r="A638" t="s">
+        <v>504</v>
+      </c>
+      <c r="B638" t="s">
+        <v>1421</v>
+      </c>
+      <c r="C638" t="s">
+        <v>10</v>
+      </c>
+      <c r="D638" t="s">
+        <v>1422</v>
+      </c>
+      <c r="E638" t="s">
+        <v>1503</v>
+      </c>
+      <c r="F638" t="s">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="639" spans="1:6">
+      <c r="A639" t="s">
+        <v>504</v>
+      </c>
+      <c r="B639" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C639" t="s">
+        <v>10</v>
+      </c>
+      <c r="D639" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E639" t="s">
+        <v>1505</v>
+      </c>
+      <c r="F639" t="s">
+        <v>1506</v>
+      </c>
+    </row>
+    <row r="640" spans="1:6">
+      <c r="A640" t="s">
+        <v>504</v>
+      </c>
+      <c r="B640" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C640" t="s">
+        <v>10</v>
+      </c>
+      <c r="D640" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E640" t="s">
+        <v>1507</v>
+      </c>
+      <c r="F640" t="s">
+        <v>1508</v>
+      </c>
+    </row>
+    <row r="641" spans="1:6">
+      <c r="A641" t="s">
+        <v>504</v>
+      </c>
+      <c r="B641" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C641" t="s">
+        <v>10</v>
+      </c>
+      <c r="D641" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E641" t="s">
+        <v>1509</v>
+      </c>
+      <c r="F641" t="s">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="642" spans="1:6">
+      <c r="A642" t="s">
+        <v>8</v>
+      </c>
+      <c r="B642" t="s">
+        <v>1367</v>
+      </c>
+      <c r="C642" t="s">
+        <v>10</v>
+      </c>
+      <c r="D642" t="s">
+        <v>1368</v>
+      </c>
+      <c r="E642" t="s">
+        <v>1511</v>
+      </c>
+      <c r="F642" t="s">
+        <v>1512</v>
+      </c>
+    </row>
+    <row r="643" spans="1:6">
+      <c r="A643" t="s">
+        <v>8</v>
+      </c>
+      <c r="B643" t="s">
+        <v>1349</v>
+      </c>
+      <c r="C643" t="s">
+        <v>10</v>
+      </c>
+      <c r="D643" t="s">
+        <v>1350</v>
+      </c>
+      <c r="E643" t="s">
+        <v>1513</v>
+      </c>
+      <c r="F643" t="s">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="644" spans="1:6">
+      <c r="A644" t="s">
+        <v>8</v>
+      </c>
+      <c r="B644" t="s">
+        <v>1359</v>
+      </c>
+      <c r="C644" t="s">
+        <v>10</v>
+      </c>
+      <c r="D644" t="s">
+        <v>1515</v>
+      </c>
+      <c r="E644" t="s">
+        <v>1516</v>
+      </c>
+      <c r="F644" t="s">
+        <v>1517</v>
+      </c>
+    </row>
+    <row r="645" spans="1:6">
+      <c r="A645" t="s">
+        <v>504</v>
+      </c>
+      <c r="B645" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C645" t="s">
+        <v>10</v>
+      </c>
+      <c r="D645" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E645" t="s">
+        <v>1518</v>
+      </c>
+      <c r="F645" t="s">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="646" spans="1:6">
+      <c r="A646" t="s">
+        <v>504</v>
+      </c>
+      <c r="B646" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C646" t="s">
+        <v>10</v>
+      </c>
+      <c r="D646" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E646" t="s">
+        <v>1520</v>
+      </c>
+      <c r="F646" t="s">
+        <v>1521</v>
+      </c>
+    </row>
+    <row r="647" spans="1:6">
+      <c r="A647" t="s">
+        <v>504</v>
+      </c>
+      <c r="B647" t="s">
+        <v>1439</v>
+      </c>
+      <c r="C647" t="s">
+        <v>10</v>
+      </c>
+      <c r="D647" t="s">
+        <v>1440</v>
+      </c>
+      <c r="E647" t="s">
+        <v>1522</v>
+      </c>
+      <c r="F647" t="s">
+        <v>1523</v>
+      </c>
+    </row>
+    <row r="648" spans="1:6">
+      <c r="A648" t="s">
+        <v>504</v>
+      </c>
+      <c r="B648" t="s">
+        <v>1405</v>
+      </c>
+      <c r="C648" t="s">
+        <v>10</v>
+      </c>
+      <c r="D648" t="s">
+        <v>1406</v>
+      </c>
+      <c r="E648" t="s">
+        <v>1524</v>
+      </c>
+      <c r="F648" t="s">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="649" spans="1:6">
+      <c r="A649" t="s">
+        <v>8</v>
+      </c>
+      <c r="B649" t="s">
+        <v>1385</v>
+      </c>
+      <c r="C649" t="s">
+        <v>10</v>
+      </c>
+      <c r="D649" t="s">
+        <v>1386</v>
+      </c>
+      <c r="E649" t="s">
+        <v>1526</v>
+      </c>
+      <c r="F649" t="s">
+        <v>1527</v>
+      </c>
+    </row>
+    <row r="650" spans="1:6">
+      <c r="A650" t="s">
+        <v>504</v>
+      </c>
+      <c r="B650" t="s">
+        <v>1417</v>
+      </c>
+      <c r="C650" t="s">
+        <v>10</v>
+      </c>
+      <c r="D650" t="s">
+        <v>1418</v>
+      </c>
+      <c r="E650" t="s">
+        <v>1528</v>
+      </c>
+      <c r="F650" t="s">
+        <v>1529</v>
+      </c>
+    </row>
+    <row r="653" spans="1:6">
+      <c r="E653" s="1" t="s">
+        <v>1530</v>
+      </c>
+      <c r="F653" s="1" t="s">
+        <v>1531</v>
       </c>
     </row>
   </sheetData>

</xml_diff>